<commit_message>
added new queries sku related info
</commit_message>
<xml_diff>
--- a/datasets/WHIsize_block_tph.xlsx
+++ b/datasets/WHIsize_block_tph.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/jesid_usf_edu/Documents/Gerdau Projects/pft/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{E76A795E-9908-1743-8BE4-AC7329BE69B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91BA2830-5DBD-AD4E-92A0-C997839C6B3B}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{E76A795E-9908-1743-8BE4-AC7329BE69B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61E9D1EA-AA2C-E94E-99AF-49AE4173430D}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="-23540" windowWidth="19560" windowHeight="15020" xr2:uid="{3215DAE6-38D8-A14D-9E7F-BA1758B64695}"/>
+    <workbookView xWindow="16200" yWindow="-16720" windowWidth="13380" windowHeight="15260" xr2:uid="{3215DAE6-38D8-A14D-9E7F-BA1758B64695}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$172</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="224">
   <si>
     <t>wc_description</t>
   </si>
@@ -772,10 +772,12 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1089,11 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C226B9-B659-3148-93FB-191C240E4220}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C153"/>
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1118,7 +1119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>53.1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>52.3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>63.63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>56.73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>54.33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>38.090000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>41.22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>50.08</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>42.3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>47.9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" hidden="1" customHeight="1">
+    <row r="25" spans="1:4" ht="17" customHeight="1">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" hidden="1" customHeight="1">
+    <row r="26" spans="1:4" ht="17" customHeight="1">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>36.78</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>31.61</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>47.3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>51.78</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>39.29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>30.03</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>40.29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>40.17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>58.88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>54.55</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>39.97</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>50.06</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>35.340000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>33.549999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>51.29</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>40.119999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>41.53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>58.52</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>38.200000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>45.7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +1959,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>54.9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -1986,7 +1987,7 @@
         <v>50.44</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>42.7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>42.9</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -2042,7 +2043,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2060,14 +2061,17 @@
       <c r="A69" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" hidden="1">
+      <c r="B69" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2075,13 +2079,13 @@
         <v>87</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D70">
-        <v>45.9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" hidden="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -2089,27 +2093,27 @@
         <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D71">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" hidden="1">
+        <v>51.7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D72">
-        <v>51.7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" hidden="1">
+        <v>21.32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -2117,13 +2121,13 @@
         <v>91</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D73">
-        <v>21.32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" hidden="1">
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -2131,27 +2135,27 @@
         <v>91</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D74">
-        <v>38.4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" hidden="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
-      </c>
-      <c r="D75">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" hidden="1">
+        <v>96</v>
+      </c>
+      <c r="D75" s="2">
+        <v>38.133658237482585</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -2159,27 +2163,25 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D76" s="2">
-        <v>38.133658237482585</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" hidden="1">
+        <v>38.339386084252681</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>4</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C77" t="s">
-        <v>97</v>
-      </c>
-      <c r="D77" s="2">
-        <v>38.339386084252681</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="C77" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" ht="17" customHeight="1">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -2187,7 +2189,7 @@
         <v>95</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -2199,7 +2201,7 @@
         <v>95</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D79" s="2"/>
     </row>
@@ -2211,23 +2213,25 @@
         <v>95</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" ht="17" customHeight="1">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>4</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" hidden="1">
+      <c r="B81" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" t="s">
+        <v>99</v>
+      </c>
+      <c r="D81">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -2235,13 +2239,13 @@
         <v>98</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D82">
-        <v>36.1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" hidden="1">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -2249,13 +2253,13 @@
         <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D83">
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" hidden="1">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -2263,13 +2267,13 @@
         <v>98</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D84">
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" hidden="1">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -2277,24 +2281,21 @@
         <v>98</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D85">
-        <v>43.9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" hidden="1">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>4</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C86" t="s">
-        <v>103</v>
-      </c>
-      <c r="D86">
-        <v>50.2</v>
+      <c r="C86" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2305,21 +2306,24 @@
         <v>98</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" hidden="1">
+      <c r="B88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -2327,13 +2331,13 @@
         <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D89">
-        <v>41.1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" hidden="1">
+        <v>44.7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -2341,13 +2345,13 @@
         <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D90">
-        <v>44.7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" hidden="1">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -2355,13 +2359,13 @@
         <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D91">
-        <v>35.1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" hidden="1">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -2369,24 +2373,21 @@
         <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D92">
-        <v>41.3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" hidden="1">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>4</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C93" t="s">
-        <v>115</v>
-      </c>
-      <c r="D93">
-        <v>23.8</v>
+      <c r="C93" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2397,21 +2398,24 @@
         <v>110</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>4</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" hidden="1">
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" t="s">
+        <v>119</v>
+      </c>
+      <c r="D95">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -2419,13 +2423,13 @@
         <v>118</v>
       </c>
       <c r="C96" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D96">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" hidden="1">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -2433,13 +2437,13 @@
         <v>118</v>
       </c>
       <c r="C97" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D97">
-        <v>48.8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" hidden="1">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -2447,13 +2451,13 @@
         <v>118</v>
       </c>
       <c r="C98" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D98">
-        <v>51.4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" hidden="1">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -2461,38 +2465,38 @@
         <v>118</v>
       </c>
       <c r="C99" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D99">
-        <v>40.1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" hidden="1">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>4</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C100" t="s">
-        <v>123</v>
+      <c r="C100" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="D100">
-        <v>30.2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" hidden="1">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>124</v>
+      <c r="C101" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="D101">
-        <v>45.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2503,21 +2507,24 @@
         <v>118</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" hidden="1">
+      <c r="B103" t="s">
+        <v>127</v>
+      </c>
+      <c r="C103" t="s">
+        <v>128</v>
+      </c>
+      <c r="D103">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -2525,13 +2532,13 @@
         <v>127</v>
       </c>
       <c r="C104" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D104">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" hidden="1">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -2539,13 +2546,13 @@
         <v>127</v>
       </c>
       <c r="C105" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D105">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" hidden="1">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -2553,13 +2560,13 @@
         <v>127</v>
       </c>
       <c r="C106" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D106">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" hidden="1">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -2567,24 +2574,21 @@
         <v>127</v>
       </c>
       <c r="C107" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D107">
-        <v>37.1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" hidden="1">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>4</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C108" t="s">
-        <v>132</v>
-      </c>
-      <c r="D108">
-        <v>38.5</v>
+      <c r="C108" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2595,21 +2599,24 @@
         <v>127</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" hidden="1">
+        <v>135</v>
+      </c>
+      <c r="B110" t="s">
+        <v>136</v>
+      </c>
+      <c r="C110" t="s">
+        <v>144</v>
+      </c>
+      <c r="D110">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>135</v>
       </c>
@@ -2617,13 +2624,13 @@
         <v>136</v>
       </c>
       <c r="C111" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D111">
-        <v>38.1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" hidden="1">
+        <v>43.86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>135</v>
       </c>
@@ -2631,13 +2638,13 @@
         <v>136</v>
       </c>
       <c r="C112" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D112">
-        <v>43.86</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" hidden="1">
+        <v>45.54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>135</v>
       </c>
@@ -2645,13 +2652,13 @@
         <v>136</v>
       </c>
       <c r="C113" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D113">
-        <v>45.54</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" hidden="1">
+        <v>64.650000000000006</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>135</v>
       </c>
@@ -2659,13 +2666,13 @@
         <v>136</v>
       </c>
       <c r="C114" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D114">
-        <v>64.650000000000006</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" hidden="1">
+        <v>28.45</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -2673,13 +2680,13 @@
         <v>136</v>
       </c>
       <c r="C115" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D115">
-        <v>28.45</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" hidden="1">
+        <v>53.54</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>135</v>
       </c>
@@ -2687,13 +2694,13 @@
         <v>136</v>
       </c>
       <c r="C116" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D116">
-        <v>53.54</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" hidden="1">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>135</v>
       </c>
@@ -2701,13 +2708,13 @@
         <v>136</v>
       </c>
       <c r="C117" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D117">
-        <v>32.799999999999997</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" hidden="1">
+        <v>56.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -2715,13 +2722,13 @@
         <v>136</v>
       </c>
       <c r="C118" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D118">
-        <v>56.4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" hidden="1">
+        <v>32.909999999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -2729,24 +2736,24 @@
         <v>136</v>
       </c>
       <c r="C119" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D119">
-        <v>32.909999999999997</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" hidden="1">
+        <v>48.29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>135</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C120" t="s">
-        <v>143</v>
+      <c r="C120" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="D120">
-        <v>48.29</v>
+        <v>29.09</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2757,7 +2764,10 @@
         <v>136</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="D121">
+        <v>37.299999999999997</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2768,21 +2778,27 @@
         <v>136</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="D122">
+        <v>51</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" hidden="1">
+      <c r="B123" t="s">
+        <v>154</v>
+      </c>
+      <c r="C123" t="s">
+        <v>150</v>
+      </c>
+      <c r="D123">
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>135</v>
       </c>
@@ -2790,13 +2806,13 @@
         <v>154</v>
       </c>
       <c r="C124" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D124">
-        <v>44.6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" hidden="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>135</v>
       </c>
@@ -2804,13 +2820,13 @@
         <v>154</v>
       </c>
       <c r="C125" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D125">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" hidden="1">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>135</v>
       </c>
@@ -2818,27 +2834,27 @@
         <v>154</v>
       </c>
       <c r="C126" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D126">
-        <v>39.200000000000003</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>135</v>
       </c>
       <c r="B127" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C127" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D127">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" hidden="1">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -2846,13 +2862,13 @@
         <v>155</v>
       </c>
       <c r="C128" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D128">
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" hidden="1">
+        <v>36.57</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -2860,13 +2876,13 @@
         <v>155</v>
       </c>
       <c r="C129" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D129">
-        <v>36.57</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" hidden="1">
+        <v>46.15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>135</v>
       </c>
@@ -2874,167 +2890,167 @@
         <v>155</v>
       </c>
       <c r="C130" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D130">
-        <v>46.15</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" hidden="1">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>135</v>
       </c>
       <c r="B131" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C131" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D131">
-        <v>45.1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" hidden="1">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>135</v>
       </c>
       <c r="B132" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C132" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D132">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" hidden="1">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C133" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D133">
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" hidden="1">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C134" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D134">
-        <v>71.2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" hidden="1">
+        <v>71.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C135" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D135">
-        <v>71.8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" hidden="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C136" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D136">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>170</v>
+      </c>
+      <c r="C137" t="s">
+        <v>176</v>
+      </c>
+      <c r="D137">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>135</v>
+      </c>
+      <c r="B138" t="s">
+        <v>164</v>
+      </c>
+      <c r="C138" t="s">
+        <v>178</v>
+      </c>
+      <c r="D138">
         <v>55</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1">
-      <c r="A137" t="s">
-        <v>135</v>
-      </c>
-      <c r="B137" t="s">
-        <v>163</v>
-      </c>
-      <c r="C137" t="s">
-        <v>175</v>
-      </c>
-      <c r="D137">
-        <v>51.6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" hidden="1">
-      <c r="A138" t="s">
-        <v>135</v>
-      </c>
-      <c r="B138" t="s">
-        <v>170</v>
-      </c>
-      <c r="C138" t="s">
-        <v>176</v>
-      </c>
-      <c r="D138">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" hidden="1">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>135</v>
       </c>
       <c r="B139" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C139" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D139">
         <v>55</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>135</v>
       </c>
       <c r="B140" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C140" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D140">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" hidden="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>135</v>
       </c>
       <c r="B141" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C141" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D141">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" hidden="1">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>135</v>
       </c>
@@ -3042,13 +3058,13 @@
         <v>180</v>
       </c>
       <c r="C142" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D142">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" hidden="1">
+        <v>43.85</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>135</v>
       </c>
@@ -3056,13 +3072,13 @@
         <v>180</v>
       </c>
       <c r="C143" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D143">
-        <v>43.85</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" hidden="1">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>135</v>
       </c>
@@ -3070,13 +3086,13 @@
         <v>180</v>
       </c>
       <c r="C144" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D144">
-        <v>58.1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" hidden="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>135</v>
       </c>
@@ -3084,13 +3100,13 @@
         <v>180</v>
       </c>
       <c r="C145" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D145">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" hidden="1">
+        <v>52.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>135</v>
       </c>
@@ -3098,13 +3114,13 @@
         <v>180</v>
       </c>
       <c r="C146" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D146">
-        <v>52.6</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" hidden="1">
+        <v>56.2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>135</v>
       </c>
@@ -3112,38 +3128,41 @@
         <v>180</v>
       </c>
       <c r="C147" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D147">
-        <v>56.2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" hidden="1">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>135</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C148" t="s">
-        <v>187</v>
+      <c r="C148" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="D148">
-        <v>27.3</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>135</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" hidden="1">
+      <c r="B149" t="s">
+        <v>189</v>
+      </c>
+      <c r="C149" t="s">
+        <v>191</v>
+      </c>
+      <c r="D149">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>135</v>
       </c>
@@ -3151,13 +3170,13 @@
         <v>189</v>
       </c>
       <c r="C150" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D150">
-        <v>29.1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" hidden="1">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>135</v>
       </c>
@@ -3165,150 +3184,153 @@
         <v>189</v>
       </c>
       <c r="C151" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D151">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" hidden="1">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>135</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C152" t="s">
-        <v>192</v>
+      <c r="C152" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="D152">
-        <v>25.8</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>135</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" hidden="1">
+      <c r="B153" t="s">
+        <v>194</v>
+      </c>
+      <c r="C153" t="s">
+        <v>195</v>
+      </c>
+      <c r="D153">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>135</v>
       </c>
       <c r="B154" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C154" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D154">
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" hidden="1">
+        <v>57.75</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>135</v>
       </c>
       <c r="B155" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C155" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D155">
-        <v>57.75</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" hidden="1">
+        <v>49.85</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>135</v>
       </c>
       <c r="B156" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C156" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D156">
-        <v>49.85</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" hidden="1">
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>135</v>
       </c>
       <c r="B157" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C157" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D157">
-        <v>46.3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" hidden="1">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>135</v>
       </c>
       <c r="B158" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C158" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D158">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>135</v>
+      </c>
+      <c r="B159" t="s">
+        <v>208</v>
+      </c>
+      <c r="C159" t="s">
+        <v>206</v>
+      </c>
+      <c r="D159">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>135</v>
+      </c>
+      <c r="B160" t="s">
+        <v>209</v>
+      </c>
+      <c r="C160" t="s">
+        <v>207</v>
+      </c>
+      <c r="D160">
+        <v>51.8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>135</v>
+      </c>
+      <c r="B161" t="s">
+        <v>210</v>
+      </c>
+      <c r="C161" t="s">
+        <v>211</v>
+      </c>
+      <c r="D161">
         <v>39.5</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1">
-      <c r="A159" t="s">
-        <v>135</v>
-      </c>
-      <c r="B159" t="s">
-        <v>204</v>
-      </c>
-      <c r="C159" t="s">
-        <v>205</v>
-      </c>
-      <c r="D159">
-        <v>47.2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" hidden="1">
-      <c r="A160" t="s">
-        <v>135</v>
-      </c>
-      <c r="B160" t="s">
-        <v>208</v>
-      </c>
-      <c r="C160" t="s">
-        <v>206</v>
-      </c>
-      <c r="D160">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" hidden="1">
-      <c r="A161" t="s">
-        <v>135</v>
-      </c>
-      <c r="B161" t="s">
-        <v>209</v>
-      </c>
-      <c r="C161" t="s">
-        <v>207</v>
-      </c>
-      <c r="D161">
-        <v>51.8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" hidden="1">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>135</v>
       </c>
@@ -3316,13 +3338,13 @@
         <v>210</v>
       </c>
       <c r="C162" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D162">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" hidden="1">
+        <v>36.549999999999997</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>135</v>
       </c>
@@ -3330,13 +3352,13 @@
         <v>210</v>
       </c>
       <c r="C163" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D163">
-        <v>36.549999999999997</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" hidden="1">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>135</v>
       </c>
@@ -3344,13 +3366,13 @@
         <v>210</v>
       </c>
       <c r="C164" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D164">
-        <v>37.200000000000003</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" hidden="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>135</v>
       </c>
@@ -3358,13 +3380,13 @@
         <v>210</v>
       </c>
       <c r="C165" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="D165">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" hidden="1">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>135</v>
       </c>
@@ -3372,13 +3394,13 @@
         <v>210</v>
       </c>
       <c r="C166" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D166">
-        <v>63.2</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" hidden="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>135</v>
       </c>
@@ -3386,13 +3408,13 @@
         <v>210</v>
       </c>
       <c r="C167" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D167">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" hidden="1">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>135</v>
       </c>
@@ -3400,27 +3422,27 @@
         <v>210</v>
       </c>
       <c r="C168" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D168">
-        <v>61.7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" hidden="1">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>135</v>
       </c>
       <c r="B169" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C169" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D169">
-        <v>41.6</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" hidden="1">
+        <v>30.86</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>135</v>
       </c>
@@ -3428,13 +3450,13 @@
         <v>219</v>
       </c>
       <c r="C170" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D170">
-        <v>30.86</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" hidden="1">
+        <v>38.49</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>135</v>
       </c>
@@ -3442,13 +3464,13 @@
         <v>219</v>
       </c>
       <c r="C171" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D171">
-        <v>38.49</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" hidden="1">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>135</v>
       </c>
@@ -3456,33 +3478,18 @@
         <v>219</v>
       </c>
       <c r="C172" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D172">
-        <v>49.2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" hidden="1">
-      <c r="A173" t="s">
-        <v>135</v>
-      </c>
-      <c r="B173" t="s">
-        <v>219</v>
-      </c>
-      <c r="C173" t="s">
-        <v>223</v>
-      </c>
-      <c r="D173">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D173" xr:uid="{02BC92E8-42B8-FF40-81FC-E7D052C55DB5}">
-    <filterColumn colId="1">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D172" xr:uid="{02BC92E8-42B8-FF40-81FC-E7D052C55DB5}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleaning up block recors, understood not identified blocks are transfered for other mill
</commit_message>
<xml_diff>
--- a/datasets/WHIsize_block_tph.xlsx
+++ b/datasets/WHIsize_block_tph.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/jesid_usf_edu/Documents/Gerdau Projects/pft/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{E76A795E-9908-1743-8BE4-AC7329BE69B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61E9D1EA-AA2C-E94E-99AF-49AE4173430D}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="8_{E76A795E-9908-1743-8BE4-AC7329BE69B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0604816-12B3-F747-B19F-2DB1E1523FF9}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="-16720" windowWidth="13380" windowHeight="15260" xr2:uid="{3215DAE6-38D8-A14D-9E7F-BA1758B64695}"/>
+    <workbookView xWindow="1760" yWindow="-19580" windowWidth="27820" windowHeight="18120" activeTab="1" xr2:uid="{3215DAE6-38D8-A14D-9E7F-BA1758B64695}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$172</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="224">
   <si>
     <t>wc_description</t>
   </si>
@@ -761,11 +762,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,14 +1097,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C226B9-B659-3148-93FB-191C240E4220}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
@@ -1109,7 +1113,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1123,7 +1127,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1137,7 +1141,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
@@ -1151,7 +1155,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -1165,7 +1169,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
@@ -1179,7 +1183,7 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
@@ -1193,7 +1197,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1207,7 +1211,7 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
@@ -1221,7 +1225,7 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -1235,7 +1239,7 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
@@ -1249,7 +1253,7 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
@@ -1263,7 +1267,7 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
@@ -1277,7 +1281,7 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -1291,7 +1295,7 @@
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
@@ -1305,7 +1309,7 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
@@ -1319,7 +1323,7 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
@@ -1333,7 +1337,7 @@
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
@@ -1347,7 +1351,7 @@
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
@@ -1361,7 +1365,7 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C19" t="s">
@@ -1375,7 +1379,7 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
@@ -1389,7 +1393,7 @@
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
@@ -1403,7 +1407,7 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
@@ -1417,7 +1421,7 @@
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C23" t="s">
@@ -1431,7 +1435,7 @@
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
@@ -1445,7 +1449,7 @@
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C25" t="s">
@@ -1459,7 +1463,7 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C26" t="s">
@@ -1473,7 +1477,7 @@
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C27" t="s">
@@ -1487,7 +1491,7 @@
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C28" t="s">
@@ -1501,7 +1505,7 @@
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C29" t="s">
@@ -1515,7 +1519,7 @@
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" t="s">
@@ -1529,7 +1533,7 @@
       <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" t="s">
@@ -1543,7 +1547,7 @@
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C32" t="s">
@@ -1557,7 +1561,7 @@
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C33" t="s">
@@ -1571,7 +1575,7 @@
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C34" t="s">
@@ -1585,7 +1589,7 @@
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C35" t="s">
@@ -1599,7 +1603,7 @@
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C36" t="s">
@@ -1613,7 +1617,7 @@
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C37" t="s">
@@ -1627,7 +1631,7 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C38" t="s">
@@ -1641,7 +1645,7 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C39" t="s">
@@ -1655,7 +1659,7 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C40" t="s">
@@ -1669,7 +1673,7 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" t="s">
@@ -1683,7 +1687,7 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C42" t="s">
@@ -1697,7 +1701,7 @@
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C43" t="s">
@@ -1711,7 +1715,7 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C44" t="s">
@@ -1725,7 +1729,7 @@
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C45" t="s">
@@ -1739,7 +1743,7 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C46" t="s">
@@ -1753,7 +1757,7 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C47" t="s">
@@ -1767,7 +1771,7 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C48" t="s">
@@ -1781,7 +1785,7 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C49" t="s">
@@ -1795,7 +1799,7 @@
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C50" t="s">
@@ -1809,7 +1813,7 @@
       <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C51" t="s">
@@ -1823,7 +1827,7 @@
       <c r="A52" t="s">
         <v>4</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C52" t="s">
@@ -1837,7 +1841,7 @@
       <c r="A53" t="s">
         <v>4</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C53" t="s">
@@ -1851,7 +1855,7 @@
       <c r="A54" t="s">
         <v>4</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C54" t="s">
@@ -1865,7 +1869,7 @@
       <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C55" t="s">
@@ -1879,7 +1883,7 @@
       <c r="A56" t="s">
         <v>4</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C56" t="s">
@@ -1893,7 +1897,7 @@
       <c r="A57" t="s">
         <v>4</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C57" t="s">
@@ -1907,7 +1911,7 @@
       <c r="A58" t="s">
         <v>4</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C58" t="s">
@@ -1921,7 +1925,7 @@
       <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C59" t="s">
@@ -1935,7 +1939,7 @@
       <c r="A60" t="s">
         <v>4</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C60" t="s">
@@ -1949,7 +1953,7 @@
       <c r="A61" t="s">
         <v>4</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C61" t="s">
@@ -1963,7 +1967,7 @@
       <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C62" t="s">
@@ -1977,7 +1981,7 @@
       <c r="A63" t="s">
         <v>4</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C63" t="s">
@@ -1991,7 +1995,7 @@
       <c r="A64" t="s">
         <v>4</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C64" t="s">
@@ -2005,7 +2009,7 @@
       <c r="A65" t="s">
         <v>4</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C65" t="s">
@@ -2019,7 +2023,7 @@
       <c r="A66" t="s">
         <v>4</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C66" t="s">
@@ -2033,7 +2037,7 @@
       <c r="A67" t="s">
         <v>4</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C67" t="s">
@@ -2047,7 +2051,7 @@
       <c r="A68" t="s">
         <v>4</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C68" t="s">
@@ -2061,7 +2065,7 @@
       <c r="A69" t="s">
         <v>4</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C69" t="s">
@@ -2075,7 +2079,7 @@
       <c r="A70" t="s">
         <v>4</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C70" t="s">
@@ -2089,7 +2093,7 @@
       <c r="A71" t="s">
         <v>4</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C71" t="s">
@@ -2103,7 +2107,7 @@
       <c r="A72" t="s">
         <v>4</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C72" t="s">
@@ -2117,7 +2121,7 @@
       <c r="A73" t="s">
         <v>4</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C73" t="s">
@@ -2131,7 +2135,7 @@
       <c r="A74" t="s">
         <v>4</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C74" t="s">
@@ -2145,7 +2149,7 @@
       <c r="A75" t="s">
         <v>4</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C75" t="s">
@@ -2159,7 +2163,7 @@
       <c r="A76" t="s">
         <v>4</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C76" t="s">
@@ -2173,7 +2177,7 @@
       <c r="A77" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -2185,7 +2189,7 @@
       <c r="A78" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -2197,7 +2201,7 @@
       <c r="A79" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2209,7 +2213,7 @@
       <c r="A80" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2221,7 +2225,7 @@
       <c r="A81" t="s">
         <v>4</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C81" t="s">
@@ -2235,7 +2239,7 @@
       <c r="A82" t="s">
         <v>4</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C82" t="s">
@@ -2249,7 +2253,7 @@
       <c r="A83" t="s">
         <v>4</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C83" t="s">
@@ -2263,7 +2267,7 @@
       <c r="A84" t="s">
         <v>4</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C84" t="s">
@@ -2277,7 +2281,7 @@
       <c r="A85" t="s">
         <v>4</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C85" t="s">
@@ -2291,7 +2295,7 @@
       <c r="A86" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -2302,7 +2306,7 @@
       <c r="A87" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2313,7 +2317,7 @@
       <c r="A88" t="s">
         <v>4</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C88" t="s">
@@ -2327,7 +2331,7 @@
       <c r="A89" t="s">
         <v>4</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C89" t="s">
@@ -2341,7 +2345,7 @@
       <c r="A90" t="s">
         <v>4</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C90" t="s">
@@ -2355,7 +2359,7 @@
       <c r="A91" t="s">
         <v>4</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C91" t="s">
@@ -2369,7 +2373,7 @@
       <c r="A92" t="s">
         <v>4</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C92" t="s">
@@ -2383,7 +2387,7 @@
       <c r="A93" t="s">
         <v>4</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -2394,7 +2398,7 @@
       <c r="A94" t="s">
         <v>4</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -2405,7 +2409,7 @@
       <c r="A95" t="s">
         <v>4</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C95" t="s">
@@ -2419,7 +2423,7 @@
       <c r="A96" t="s">
         <v>4</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C96" t="s">
@@ -2433,7 +2437,7 @@
       <c r="A97" t="s">
         <v>4</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C97" t="s">
@@ -2447,7 +2451,7 @@
       <c r="A98" t="s">
         <v>4</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C98" t="s">
@@ -2461,7 +2465,7 @@
       <c r="A99" t="s">
         <v>4</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C99" t="s">
@@ -2475,7 +2479,7 @@
       <c r="A100" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -2489,7 +2493,7 @@
       <c r="A101" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -2503,7 +2507,7 @@
       <c r="A102" t="s">
         <v>4</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -2514,7 +2518,7 @@
       <c r="A103" t="s">
         <v>4</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C103" t="s">
@@ -2528,7 +2532,7 @@
       <c r="A104" t="s">
         <v>4</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C104" t="s">
@@ -2542,7 +2546,7 @@
       <c r="A105" t="s">
         <v>4</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C105" t="s">
@@ -2556,7 +2560,7 @@
       <c r="A106" t="s">
         <v>4</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C106" t="s">
@@ -2570,7 +2574,7 @@
       <c r="A107" t="s">
         <v>4</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="4" t="s">
         <v>127</v>
       </c>
       <c r="C107" t="s">
@@ -2584,7 +2588,7 @@
       <c r="A108" t="s">
         <v>4</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -2595,7 +2599,7 @@
       <c r="A109" t="s">
         <v>4</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -2606,7 +2610,7 @@
       <c r="A110" t="s">
         <v>135</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C110" t="s">
@@ -2620,7 +2624,7 @@
       <c r="A111" t="s">
         <v>135</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C111" t="s">
@@ -2634,7 +2638,7 @@
       <c r="A112" t="s">
         <v>135</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C112" t="s">
@@ -2648,7 +2652,7 @@
       <c r="A113" t="s">
         <v>135</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C113" t="s">
@@ -2662,7 +2666,7 @@
       <c r="A114" t="s">
         <v>135</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C114" t="s">
@@ -2676,7 +2680,7 @@
       <c r="A115" t="s">
         <v>135</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C115" t="s">
@@ -2690,7 +2694,7 @@
       <c r="A116" t="s">
         <v>135</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C116" t="s">
@@ -2704,7 +2708,7 @@
       <c r="A117" t="s">
         <v>135</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C117" t="s">
@@ -2718,7 +2722,7 @@
       <c r="A118" t="s">
         <v>135</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C118" t="s">
@@ -2732,7 +2736,7 @@
       <c r="A119" t="s">
         <v>135</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C119" t="s">
@@ -2746,7 +2750,7 @@
       <c r="A120" t="s">
         <v>135</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -2760,7 +2764,7 @@
       <c r="A121" t="s">
         <v>135</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -2774,7 +2778,7 @@
       <c r="A122" t="s">
         <v>135</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -2788,7 +2792,7 @@
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="4" t="s">
         <v>154</v>
       </c>
       <c r="C123" t="s">
@@ -2802,7 +2806,7 @@
       <c r="A124" t="s">
         <v>135</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="4" t="s">
         <v>154</v>
       </c>
       <c r="C124" t="s">
@@ -2816,7 +2820,7 @@
       <c r="A125" t="s">
         <v>135</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="4" t="s">
         <v>154</v>
       </c>
       <c r="C125" t="s">
@@ -2830,7 +2834,7 @@
       <c r="A126" t="s">
         <v>135</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="4" t="s">
         <v>154</v>
       </c>
       <c r="C126" t="s">
@@ -2844,7 +2848,7 @@
       <c r="A127" t="s">
         <v>135</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C127" t="s">
@@ -2858,7 +2862,7 @@
       <c r="A128" t="s">
         <v>135</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C128" t="s">
@@ -2872,7 +2876,7 @@
       <c r="A129" t="s">
         <v>135</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C129" t="s">
@@ -2886,7 +2890,7 @@
       <c r="A130" t="s">
         <v>135</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C130" t="s">
@@ -2900,7 +2904,7 @@
       <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="4" t="s">
         <v>160</v>
       </c>
       <c r="C131" t="s">
@@ -2914,7 +2918,7 @@
       <c r="A132" t="s">
         <v>135</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="4" t="s">
         <v>167</v>
       </c>
       <c r="C132" t="s">
@@ -2928,7 +2932,7 @@
       <c r="A133" t="s">
         <v>135</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="4" t="s">
         <v>168</v>
       </c>
       <c r="C133" t="s">
@@ -2942,7 +2946,7 @@
       <c r="A134" t="s">
         <v>135</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C134" t="s">
@@ -2956,7 +2960,7 @@
       <c r="A135" t="s">
         <v>135</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="4" t="s">
         <v>162</v>
       </c>
       <c r="C135" t="s">
@@ -2970,7 +2974,7 @@
       <c r="A136" t="s">
         <v>135</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="4" t="s">
         <v>163</v>
       </c>
       <c r="C136" t="s">
@@ -2984,7 +2988,7 @@
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="4" t="s">
         <v>170</v>
       </c>
       <c r="C137" t="s">
@@ -2998,7 +3002,7 @@
       <c r="A138" t="s">
         <v>135</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="4" t="s">
         <v>164</v>
       </c>
       <c r="C138" t="s">
@@ -3012,7 +3016,7 @@
       <c r="A139" t="s">
         <v>135</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="4" t="s">
         <v>165</v>
       </c>
       <c r="C139" t="s">
@@ -3026,7 +3030,7 @@
       <c r="A140" t="s">
         <v>135</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C140" t="s">
@@ -3040,7 +3044,7 @@
       <c r="A141" t="s">
         <v>135</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C141" t="s">
@@ -3054,7 +3058,7 @@
       <c r="A142" t="s">
         <v>135</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C142" t="s">
@@ -3068,7 +3072,7 @@
       <c r="A143" t="s">
         <v>135</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C143" t="s">
@@ -3082,7 +3086,7 @@
       <c r="A144" t="s">
         <v>135</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C144" t="s">
@@ -3096,7 +3100,7 @@
       <c r="A145" t="s">
         <v>135</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C145" t="s">
@@ -3110,7 +3114,7 @@
       <c r="A146" t="s">
         <v>135</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C146" t="s">
@@ -3124,7 +3128,7 @@
       <c r="A147" t="s">
         <v>135</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="4" t="s">
         <v>180</v>
       </c>
       <c r="C147" t="s">
@@ -3138,7 +3142,7 @@
       <c r="A148" t="s">
         <v>135</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="5" t="s">
         <v>180</v>
       </c>
       <c r="C148" s="1" t="s">
@@ -3152,7 +3156,7 @@
       <c r="A149" t="s">
         <v>135</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="4" t="s">
         <v>189</v>
       </c>
       <c r="C149" t="s">
@@ -3166,7 +3170,7 @@
       <c r="A150" t="s">
         <v>135</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="4" t="s">
         <v>189</v>
       </c>
       <c r="C150" t="s">
@@ -3180,7 +3184,7 @@
       <c r="A151" t="s">
         <v>135</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="4" t="s">
         <v>189</v>
       </c>
       <c r="C151" t="s">
@@ -3194,7 +3198,7 @@
       <c r="A152" t="s">
         <v>135</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="5" t="s">
         <v>189</v>
       </c>
       <c r="C152" s="1" t="s">
@@ -3208,7 +3212,7 @@
       <c r="A153" t="s">
         <v>135</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="4" t="s">
         <v>194</v>
       </c>
       <c r="C153" t="s">
@@ -3222,7 +3226,7 @@
       <c r="A154" t="s">
         <v>135</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="4" t="s">
         <v>200</v>
       </c>
       <c r="C154" t="s">
@@ -3236,7 +3240,7 @@
       <c r="A155" t="s">
         <v>135</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="4" t="s">
         <v>201</v>
       </c>
       <c r="C155" t="s">
@@ -3250,7 +3254,7 @@
       <c r="A156" t="s">
         <v>135</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="4" t="s">
         <v>202</v>
       </c>
       <c r="C156" t="s">
@@ -3264,7 +3268,7 @@
       <c r="A157" t="s">
         <v>135</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="4" t="s">
         <v>203</v>
       </c>
       <c r="C157" t="s">
@@ -3278,7 +3282,7 @@
       <c r="A158" t="s">
         <v>135</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="4" t="s">
         <v>204</v>
       </c>
       <c r="C158" t="s">
@@ -3292,7 +3296,7 @@
       <c r="A159" t="s">
         <v>135</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="4" t="s">
         <v>208</v>
       </c>
       <c r="C159" t="s">
@@ -3306,7 +3310,7 @@
       <c r="A160" t="s">
         <v>135</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="4" t="s">
         <v>209</v>
       </c>
       <c r="C160" t="s">
@@ -3320,7 +3324,7 @@
       <c r="A161" t="s">
         <v>135</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C161" t="s">
@@ -3334,7 +3338,7 @@
       <c r="A162" t="s">
         <v>135</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C162" t="s">
@@ -3348,7 +3352,7 @@
       <c r="A163" t="s">
         <v>135</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C163" t="s">
@@ -3362,7 +3366,7 @@
       <c r="A164" t="s">
         <v>135</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C164" t="s">
@@ -3376,7 +3380,7 @@
       <c r="A165" t="s">
         <v>135</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C165" t="s">
@@ -3390,7 +3394,7 @@
       <c r="A166" t="s">
         <v>135</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C166" t="s">
@@ -3404,7 +3408,7 @@
       <c r="A167" t="s">
         <v>135</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C167" t="s">
@@ -3418,7 +3422,7 @@
       <c r="A168" t="s">
         <v>135</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C168" t="s">
@@ -3432,7 +3436,7 @@
       <c r="A169" t="s">
         <v>135</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="4" t="s">
         <v>219</v>
       </c>
       <c r="C169" t="s">
@@ -3446,7 +3450,7 @@
       <c r="A170" t="s">
         <v>135</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="4" t="s">
         <v>219</v>
       </c>
       <c r="C170" t="s">
@@ -3460,7 +3464,7 @@
       <c r="A171" t="s">
         <v>135</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="4" t="s">
         <v>219</v>
       </c>
       <c r="C171" t="s">
@@ -3474,7 +3478,7 @@
       <c r="A172" t="s">
         <v>135</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="4" t="s">
         <v>219</v>
       </c>
       <c r="C172" t="s">
@@ -3492,4 +3496,634 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B2E9C6-5998-8241-8C07-18530F804FB0}">
+  <dimension ref="B1:B172"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53"/>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54"/>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58"/>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68"/>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75"/>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76"/>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79"/>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89"/>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90"/>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91"/>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92"/>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93"/>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94"/>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95"/>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96"/>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97"/>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98"/>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99"/>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100"/>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103"/>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104"/>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105"/>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106"/>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107"/>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108"/>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109"/>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110"/>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111"/>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112"/>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113"/>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114"/>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115"/>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116"/>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117"/>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118"/>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119"/>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120"/>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121"/>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122"/>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123"/>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124"/>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125"/>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126"/>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127"/>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128"/>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129"/>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130"/>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131"/>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132"/>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133"/>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134"/>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135"/>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136"/>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137"/>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138"/>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139"/>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140"/>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141"/>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142"/>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143"/>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144"/>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145"/>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146"/>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147"/>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148"/>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149"/>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150"/>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151"/>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152"/>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153"/>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154"/>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155"/>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156"/>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157"/>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158"/>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159"/>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160"/>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161"/>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162"/>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163"/>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164"/>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165"/>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166"/>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167"/>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168"/>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169"/>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170"/>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171"/>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>